<commit_message>
More detail to Point 5 and 6
</commit_message>
<xml_diff>
--- a/Gantt-Diagramm.xlsx
+++ b/Gantt-Diagramm.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flxti\Dropbox\UNI\2023\Projekt Intelligente Systeme\AWP_2023\AWP_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAEB3AA8-F95D-4873-8829-13363CD3B4DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14B64490-E446-4E15-86E7-4A1F6BBA2593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="1" r:id="rId1"/>
+    <sheet name="Felix" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
   <si>
     <t>KW18</t>
   </si>
@@ -125,6 +126,48 @@
   </si>
   <si>
     <t>0. Entwicklungsumgebung einrichten (Codestyle, Git, Markdown)</t>
+  </si>
+  <si>
+    <t>Untersuchung und Auswahl geeigneter Frameworks und Tools für die mobile Entwicklung</t>
+  </si>
+  <si>
+    <t>Erstellung von UI-Designs für die mobile Anwendung</t>
+  </si>
+  <si>
+    <t>Integration der Iris-Scanner-Software in die mobile Anwendung</t>
+  </si>
+  <si>
+    <t>Implementierung der Funktionalität zur Anzeige von Warnsignalen bei erkanntem Sekundenschlaf</t>
+  </si>
+  <si>
+    <t>Integration der mobilen Anwendung mit anderen relevanten Systemen (z.B. Backend-Systemen)</t>
+  </si>
+  <si>
+    <t>Integration von Funktionen zur Datenspeicherung und -analyse (z.B. Daten zu erkanntem Sekundenschlaf und Augenparameter)</t>
+  </si>
+  <si>
+    <t>Implementierung von Funktionen zur Aufzeichnung und Verarbeitung von Bildern der Frontalansichten des Gesichts</t>
+  </si>
+  <si>
+    <t>Implementierung von Funktionen zur Analyse von Augenparametern (z.B. Pupillengröße und Entfernung der Augenlieder zueinander)</t>
+  </si>
+  <si>
+    <t>Erstellung von Testfällen und Durchführung von Tests der mobilen Anwendung (z.B. Funktionalitätstests, Usability-Tests, Performance-Tests)</t>
+  </si>
+  <si>
+    <t>Analyse und Optimierung der Genauigkeit des Iris-Scanners durch Anpassung der Algorithmen und Berücksichtigung physiologischer Zusammenhänge</t>
+  </si>
+  <si>
+    <t>Optimierung der Speicherverwaltung und -nutzung, um die Leistung und Skalierbarkeit der Anwendung zu verbessern</t>
+  </si>
+  <si>
+    <t>Verbesserung der Benutzerfreundlichkeit durch Implementierung von Funktionen wie Tutorials, Hinweisen und Feedbackmechanismen</t>
+  </si>
+  <si>
+    <t>Integration von Funktionen zur Fehlerbehebung und Überwachung (z.B. Logging und Benachrichtigungen bei Fehlern)</t>
+  </si>
+  <si>
+    <t>Durchführung von Nutzertests und Analyse des Nutzungsverhaltens zur Identifizierung von Verbesserungsmöglichkeiten und Optimierung der Anwendung.</t>
   </si>
 </sst>
 </file>
@@ -134,7 +177,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,6 +203,14 @@
       <color rgb="FF5B9BD5"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -448,7 +499,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="1" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -490,56 +541,11 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -580,12 +586,62 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -893,13 +949,13 @@
   </sheetPr>
   <dimension ref="A1:BU20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A5" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="107.5703125" style="45" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="107.5703125" style="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="14" width="13.5703125" style="10" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="13.5703125" style="14" bestFit="1" customWidth="1"/>
@@ -910,185 +966,185 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:73" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="15" t="s">
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="15" t="s">
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="17"/>
-      <c r="V1" s="15" t="s">
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="W1" s="16"/>
-      <c r="X1" s="16"/>
-      <c r="Y1" s="16"/>
-      <c r="Z1" s="16"/>
-      <c r="AA1" s="16"/>
-      <c r="AB1" s="17"/>
-      <c r="AC1" s="15" t="s">
+      <c r="W1" s="31"/>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
+      <c r="AA1" s="31"/>
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="AD1" s="16"/>
-      <c r="AE1" s="16"/>
-      <c r="AF1" s="16"/>
-      <c r="AG1" s="16"/>
-      <c r="AH1" s="16"/>
-      <c r="AI1" s="17"/>
-      <c r="AJ1" s="15" t="s">
+      <c r="AD1" s="31"/>
+      <c r="AE1" s="31"/>
+      <c r="AF1" s="31"/>
+      <c r="AG1" s="31"/>
+      <c r="AH1" s="31"/>
+      <c r="AI1" s="32"/>
+      <c r="AJ1" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="AK1" s="16"/>
-      <c r="AL1" s="16"/>
-      <c r="AM1" s="16"/>
-      <c r="AN1" s="16"/>
-      <c r="AO1" s="16"/>
-      <c r="AP1" s="17"/>
-      <c r="AQ1" s="15" t="s">
+      <c r="AK1" s="31"/>
+      <c r="AL1" s="31"/>
+      <c r="AM1" s="31"/>
+      <c r="AN1" s="31"/>
+      <c r="AO1" s="31"/>
+      <c r="AP1" s="32"/>
+      <c r="AQ1" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="AR1" s="16"/>
-      <c r="AS1" s="16"/>
-      <c r="AT1" s="16"/>
-      <c r="AU1" s="16"/>
-      <c r="AV1" s="16"/>
-      <c r="AW1" s="17"/>
-      <c r="AX1" s="15" t="s">
+      <c r="AR1" s="31"/>
+      <c r="AS1" s="31"/>
+      <c r="AT1" s="31"/>
+      <c r="AU1" s="31"/>
+      <c r="AV1" s="31"/>
+      <c r="AW1" s="32"/>
+      <c r="AX1" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="AY1" s="16"/>
-      <c r="AZ1" s="16"/>
-      <c r="BA1" s="16"/>
-      <c r="BB1" s="16"/>
-      <c r="BC1" s="16"/>
-      <c r="BD1" s="17"/>
-      <c r="BE1" s="15" t="s">
+      <c r="AY1" s="31"/>
+      <c r="AZ1" s="31"/>
+      <c r="BA1" s="31"/>
+      <c r="BB1" s="31"/>
+      <c r="BC1" s="31"/>
+      <c r="BD1" s="32"/>
+      <c r="BE1" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="BF1" s="16"/>
-      <c r="BG1" s="16"/>
-      <c r="BH1" s="16"/>
-      <c r="BI1" s="16"/>
-      <c r="BJ1" s="16"/>
-      <c r="BK1" s="17"/>
-      <c r="BL1" s="15" t="s">
+      <c r="BF1" s="31"/>
+      <c r="BG1" s="31"/>
+      <c r="BH1" s="31"/>
+      <c r="BI1" s="31"/>
+      <c r="BJ1" s="31"/>
+      <c r="BK1" s="32"/>
+      <c r="BL1" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="BM1" s="16"/>
-      <c r="BN1" s="16"/>
-      <c r="BO1" s="16"/>
-      <c r="BP1" s="16"/>
-      <c r="BQ1" s="16"/>
-      <c r="BR1" s="17"/>
-      <c r="BS1" s="15" t="s">
+      <c r="BM1" s="31"/>
+      <c r="BN1" s="31"/>
+      <c r="BO1" s="31"/>
+      <c r="BP1" s="31"/>
+      <c r="BQ1" s="31"/>
+      <c r="BR1" s="32"/>
+      <c r="BS1" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="BT1" s="16"/>
-      <c r="BU1" s="17"/>
+      <c r="BT1" s="31"/>
+      <c r="BU1" s="32"/>
     </row>
     <row r="2" spans="1:73" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="21" t="s">
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="R2" s="22"/>
-      <c r="S2" s="22"/>
-      <c r="T2" s="22"/>
-      <c r="U2" s="22"/>
-      <c r="V2" s="22"/>
-      <c r="W2" s="22"/>
-      <c r="X2" s="22"/>
-      <c r="Y2" s="22"/>
-      <c r="Z2" s="22"/>
-      <c r="AA2" s="22"/>
-      <c r="AB2" s="22"/>
-      <c r="AC2" s="22"/>
-      <c r="AD2" s="23"/>
-      <c r="AE2" s="24" t="s">
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37"/>
+      <c r="V2" s="37"/>
+      <c r="W2" s="37"/>
+      <c r="X2" s="37"/>
+      <c r="Y2" s="37"/>
+      <c r="Z2" s="37"/>
+      <c r="AA2" s="37"/>
+      <c r="AB2" s="37"/>
+      <c r="AC2" s="37"/>
+      <c r="AD2" s="38"/>
+      <c r="AE2" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="AF2" s="25"/>
-      <c r="AG2" s="25"/>
-      <c r="AH2" s="25"/>
-      <c r="AI2" s="25"/>
-      <c r="AJ2" s="25"/>
-      <c r="AK2" s="25"/>
-      <c r="AL2" s="25"/>
-      <c r="AM2" s="25"/>
-      <c r="AN2" s="25"/>
-      <c r="AO2" s="25"/>
-      <c r="AP2" s="25"/>
-      <c r="AQ2" s="25"/>
-      <c r="AR2" s="26"/>
-      <c r="AS2" s="27" t="s">
+      <c r="AF2" s="40"/>
+      <c r="AG2" s="40"/>
+      <c r="AH2" s="40"/>
+      <c r="AI2" s="40"/>
+      <c r="AJ2" s="40"/>
+      <c r="AK2" s="40"/>
+      <c r="AL2" s="40"/>
+      <c r="AM2" s="40"/>
+      <c r="AN2" s="40"/>
+      <c r="AO2" s="40"/>
+      <c r="AP2" s="40"/>
+      <c r="AQ2" s="40"/>
+      <c r="AR2" s="41"/>
+      <c r="AS2" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="AT2" s="28"/>
-      <c r="AU2" s="28"/>
-      <c r="AV2" s="28"/>
-      <c r="AW2" s="28"/>
-      <c r="AX2" s="28"/>
-      <c r="AY2" s="28"/>
-      <c r="AZ2" s="28"/>
-      <c r="BA2" s="28"/>
-      <c r="BB2" s="28"/>
-      <c r="BC2" s="28"/>
-      <c r="BD2" s="28"/>
-      <c r="BE2" s="28"/>
-      <c r="BF2" s="29"/>
-      <c r="BG2" s="30" t="s">
+      <c r="AT2" s="43"/>
+      <c r="AU2" s="43"/>
+      <c r="AV2" s="43"/>
+      <c r="AW2" s="43"/>
+      <c r="AX2" s="43"/>
+      <c r="AY2" s="43"/>
+      <c r="AZ2" s="43"/>
+      <c r="BA2" s="43"/>
+      <c r="BB2" s="43"/>
+      <c r="BC2" s="43"/>
+      <c r="BD2" s="43"/>
+      <c r="BE2" s="43"/>
+      <c r="BF2" s="44"/>
+      <c r="BG2" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="BH2" s="31"/>
-      <c r="BI2" s="31"/>
-      <c r="BJ2" s="31"/>
-      <c r="BK2" s="31"/>
-      <c r="BL2" s="31"/>
-      <c r="BM2" s="31"/>
-      <c r="BN2" s="31"/>
-      <c r="BO2" s="31"/>
-      <c r="BP2" s="31"/>
-      <c r="BQ2" s="31"/>
-      <c r="BR2" s="31"/>
-      <c r="BS2" s="31"/>
-      <c r="BT2" s="31"/>
+      <c r="BH2" s="46"/>
+      <c r="BI2" s="46"/>
+      <c r="BJ2" s="46"/>
+      <c r="BK2" s="46"/>
+      <c r="BL2" s="46"/>
+      <c r="BM2" s="46"/>
+      <c r="BN2" s="46"/>
+      <c r="BO2" s="46"/>
+      <c r="BP2" s="46"/>
+      <c r="BQ2" s="46"/>
+      <c r="BR2" s="46"/>
+      <c r="BS2" s="46"/>
+      <c r="BT2" s="46"/>
       <c r="BU2" s="1"/>
     </row>
     <row r="3" spans="1:73" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1316,477 +1372,477 @@
         <v>28</v>
       </c>
       <c r="C4" s="9"/>
-      <c r="O4" s="32" t="s">
+      <c r="O4" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="P4" s="33"/>
+      <c r="P4" s="18"/>
       <c r="Q4" s="11"/>
-      <c r="AQ4" s="32" t="s">
+      <c r="AQ4" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="AR4" s="33"/>
+      <c r="AR4" s="18"/>
       <c r="AS4" s="11"/>
-      <c r="BE4" s="32" t="s">
+      <c r="BE4" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="BF4" s="33"/>
-      <c r="BG4" s="38" t="s">
+      <c r="BF4" s="18"/>
+      <c r="BG4" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="BH4" s="39"/>
-      <c r="BI4" s="39"/>
-      <c r="BJ4" s="39"/>
-      <c r="BK4" s="39"/>
-      <c r="BL4" s="39"/>
-      <c r="BM4" s="39"/>
-      <c r="BN4" s="39"/>
-      <c r="BO4" s="39"/>
-      <c r="BP4" s="39"/>
-      <c r="BQ4" s="39"/>
-      <c r="BR4" s="39"/>
-      <c r="BS4" s="39"/>
-      <c r="BT4" s="33"/>
-      <c r="BU4" s="42" t="s">
+      <c r="BH4" s="24"/>
+      <c r="BI4" s="24"/>
+      <c r="BJ4" s="24"/>
+      <c r="BK4" s="24"/>
+      <c r="BL4" s="24"/>
+      <c r="BM4" s="24"/>
+      <c r="BN4" s="24"/>
+      <c r="BO4" s="24"/>
+      <c r="BP4" s="24"/>
+      <c r="BQ4" s="24"/>
+      <c r="BR4" s="24"/>
+      <c r="BS4" s="24"/>
+      <c r="BT4" s="18"/>
+      <c r="BU4" s="27" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:73" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="15" t="s">
         <v>21</v>
       </c>
       <c r="B5" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="11"/>
-      <c r="O5" s="34"/>
-      <c r="P5" s="35"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="20"/>
       <c r="Q5" s="11"/>
-      <c r="AQ5" s="34"/>
-      <c r="AR5" s="35"/>
+      <c r="AQ5" s="19"/>
+      <c r="AR5" s="20"/>
       <c r="AS5" s="11"/>
-      <c r="BE5" s="34"/>
-      <c r="BF5" s="35"/>
-      <c r="BG5" s="40"/>
-      <c r="BH5" s="34"/>
-      <c r="BI5" s="34"/>
-      <c r="BJ5" s="34"/>
-      <c r="BK5" s="34"/>
-      <c r="BL5" s="34"/>
-      <c r="BM5" s="34"/>
-      <c r="BN5" s="34"/>
-      <c r="BO5" s="34"/>
-      <c r="BP5" s="34"/>
-      <c r="BQ5" s="34"/>
-      <c r="BR5" s="34"/>
-      <c r="BS5" s="34"/>
-      <c r="BT5" s="35"/>
-      <c r="BU5" s="43"/>
+      <c r="BE5" s="19"/>
+      <c r="BF5" s="20"/>
+      <c r="BG5" s="25"/>
+      <c r="BH5" s="19"/>
+      <c r="BI5" s="19"/>
+      <c r="BJ5" s="19"/>
+      <c r="BK5" s="19"/>
+      <c r="BL5" s="19"/>
+      <c r="BM5" s="19"/>
+      <c r="BN5" s="19"/>
+      <c r="BO5" s="19"/>
+      <c r="BP5" s="19"/>
+      <c r="BQ5" s="19"/>
+      <c r="BR5" s="19"/>
+      <c r="BS5" s="19"/>
+      <c r="BT5" s="20"/>
+      <c r="BU5" s="28"/>
     </row>
     <row r="6" spans="1:73" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="15" t="s">
         <v>22</v>
       </c>
       <c r="B6" t="s">
         <v>33</v>
       </c>
       <c r="C6" s="11"/>
-      <c r="O6" s="34"/>
-      <c r="P6" s="35"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="20"/>
       <c r="Q6" s="11"/>
-      <c r="AQ6" s="34"/>
-      <c r="AR6" s="35"/>
+      <c r="AQ6" s="19"/>
+      <c r="AR6" s="20"/>
       <c r="AS6" s="11"/>
-      <c r="BE6" s="34"/>
-      <c r="BF6" s="35"/>
-      <c r="BG6" s="40"/>
-      <c r="BH6" s="34"/>
-      <c r="BI6" s="34"/>
-      <c r="BJ6" s="34"/>
-      <c r="BK6" s="34"/>
-      <c r="BL6" s="34"/>
-      <c r="BM6" s="34"/>
-      <c r="BN6" s="34"/>
-      <c r="BO6" s="34"/>
-      <c r="BP6" s="34"/>
-      <c r="BQ6" s="34"/>
-      <c r="BR6" s="34"/>
-      <c r="BS6" s="34"/>
-      <c r="BT6" s="35"/>
-      <c r="BU6" s="43"/>
+      <c r="BE6" s="19"/>
+      <c r="BF6" s="20"/>
+      <c r="BG6" s="25"/>
+      <c r="BH6" s="19"/>
+      <c r="BI6" s="19"/>
+      <c r="BJ6" s="19"/>
+      <c r="BK6" s="19"/>
+      <c r="BL6" s="19"/>
+      <c r="BM6" s="19"/>
+      <c r="BN6" s="19"/>
+      <c r="BO6" s="19"/>
+      <c r="BP6" s="19"/>
+      <c r="BQ6" s="19"/>
+      <c r="BR6" s="19"/>
+      <c r="BS6" s="19"/>
+      <c r="BT6" s="20"/>
+      <c r="BU6" s="28"/>
     </row>
     <row r="7" spans="1:73" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B7" t="s">
         <v>33</v>
       </c>
       <c r="C7" s="11"/>
-      <c r="O7" s="34"/>
-      <c r="P7" s="35"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="20"/>
       <c r="Q7" s="11"/>
-      <c r="AQ7" s="34"/>
-      <c r="AR7" s="35"/>
+      <c r="AQ7" s="19"/>
+      <c r="AR7" s="20"/>
       <c r="AS7" s="11"/>
-      <c r="BE7" s="34"/>
-      <c r="BF7" s="35"/>
-      <c r="BG7" s="40"/>
-      <c r="BH7" s="34"/>
-      <c r="BI7" s="34"/>
-      <c r="BJ7" s="34"/>
-      <c r="BK7" s="34"/>
-      <c r="BL7" s="34"/>
-      <c r="BM7" s="34"/>
-      <c r="BN7" s="34"/>
-      <c r="BO7" s="34"/>
-      <c r="BP7" s="34"/>
-      <c r="BQ7" s="34"/>
-      <c r="BR7" s="34"/>
-      <c r="BS7" s="34"/>
-      <c r="BT7" s="35"/>
-      <c r="BU7" s="43"/>
+      <c r="BE7" s="19"/>
+      <c r="BF7" s="20"/>
+      <c r="BG7" s="25"/>
+      <c r="BH7" s="19"/>
+      <c r="BI7" s="19"/>
+      <c r="BJ7" s="19"/>
+      <c r="BK7" s="19"/>
+      <c r="BL7" s="19"/>
+      <c r="BM7" s="19"/>
+      <c r="BN7" s="19"/>
+      <c r="BO7" s="19"/>
+      <c r="BP7" s="19"/>
+      <c r="BQ7" s="19"/>
+      <c r="BR7" s="19"/>
+      <c r="BS7" s="19"/>
+      <c r="BT7" s="20"/>
+      <c r="BU7" s="28"/>
     </row>
     <row r="8" spans="1:73" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="15" t="s">
         <v>24</v>
       </c>
       <c r="B8" t="s">
         <v>32</v>
       </c>
       <c r="C8" s="11"/>
-      <c r="O8" s="34"/>
-      <c r="P8" s="35"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="20"/>
       <c r="Q8" s="11"/>
-      <c r="AQ8" s="34"/>
-      <c r="AR8" s="35"/>
+      <c r="AQ8" s="19"/>
+      <c r="AR8" s="20"/>
       <c r="AS8" s="11"/>
-      <c r="BE8" s="34"/>
-      <c r="BF8" s="35"/>
-      <c r="BG8" s="40"/>
-      <c r="BH8" s="34"/>
-      <c r="BI8" s="34"/>
-      <c r="BJ8" s="34"/>
-      <c r="BK8" s="34"/>
-      <c r="BL8" s="34"/>
-      <c r="BM8" s="34"/>
-      <c r="BN8" s="34"/>
-      <c r="BO8" s="34"/>
-      <c r="BP8" s="34"/>
-      <c r="BQ8" s="34"/>
-      <c r="BR8" s="34"/>
-      <c r="BS8" s="34"/>
-      <c r="BT8" s="35"/>
-      <c r="BU8" s="43"/>
+      <c r="BE8" s="19"/>
+      <c r="BF8" s="20"/>
+      <c r="BG8" s="25"/>
+      <c r="BH8" s="19"/>
+      <c r="BI8" s="19"/>
+      <c r="BJ8" s="19"/>
+      <c r="BK8" s="19"/>
+      <c r="BL8" s="19"/>
+      <c r="BM8" s="19"/>
+      <c r="BN8" s="19"/>
+      <c r="BO8" s="19"/>
+      <c r="BP8" s="19"/>
+      <c r="BQ8" s="19"/>
+      <c r="BR8" s="19"/>
+      <c r="BS8" s="19"/>
+      <c r="BT8" s="20"/>
+      <c r="BU8" s="28"/>
     </row>
     <row r="9" spans="1:73" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="15" t="s">
         <v>25</v>
       </c>
       <c r="B9" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="11"/>
-      <c r="O9" s="34"/>
-      <c r="P9" s="35"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="20"/>
       <c r="Q9" s="11"/>
-      <c r="AQ9" s="34"/>
-      <c r="AR9" s="35"/>
+      <c r="AQ9" s="19"/>
+      <c r="AR9" s="20"/>
       <c r="AS9" s="11"/>
-      <c r="BE9" s="34"/>
-      <c r="BF9" s="35"/>
-      <c r="BG9" s="40"/>
-      <c r="BH9" s="34"/>
-      <c r="BI9" s="34"/>
-      <c r="BJ9" s="34"/>
-      <c r="BK9" s="34"/>
-      <c r="BL9" s="34"/>
-      <c r="BM9" s="34"/>
-      <c r="BN9" s="34"/>
-      <c r="BO9" s="34"/>
-      <c r="BP9" s="34"/>
-      <c r="BQ9" s="34"/>
-      <c r="BR9" s="34"/>
-      <c r="BS9" s="34"/>
-      <c r="BT9" s="35"/>
-      <c r="BU9" s="43"/>
+      <c r="BE9" s="19"/>
+      <c r="BF9" s="20"/>
+      <c r="BG9" s="25"/>
+      <c r="BH9" s="19"/>
+      <c r="BI9" s="19"/>
+      <c r="BJ9" s="19"/>
+      <c r="BK9" s="19"/>
+      <c r="BL9" s="19"/>
+      <c r="BM9" s="19"/>
+      <c r="BN9" s="19"/>
+      <c r="BO9" s="19"/>
+      <c r="BP9" s="19"/>
+      <c r="BQ9" s="19"/>
+      <c r="BR9" s="19"/>
+      <c r="BS9" s="19"/>
+      <c r="BT9" s="20"/>
+      <c r="BU9" s="28"/>
     </row>
     <row r="10" spans="1:73" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="15" t="s">
         <v>26</v>
       </c>
       <c r="B10" t="s">
         <v>30</v>
       </c>
       <c r="C10" s="11"/>
-      <c r="O10" s="34"/>
-      <c r="P10" s="35"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="20"/>
       <c r="Q10" s="11"/>
-      <c r="AQ10" s="34"/>
-      <c r="AR10" s="35"/>
+      <c r="AQ10" s="19"/>
+      <c r="AR10" s="20"/>
       <c r="AS10" s="11"/>
-      <c r="BE10" s="34"/>
-      <c r="BF10" s="35"/>
-      <c r="BG10" s="40"/>
-      <c r="BH10" s="34"/>
-      <c r="BI10" s="34"/>
-      <c r="BJ10" s="34"/>
-      <c r="BK10" s="34"/>
-      <c r="BL10" s="34"/>
-      <c r="BM10" s="34"/>
-      <c r="BN10" s="34"/>
-      <c r="BO10" s="34"/>
-      <c r="BP10" s="34"/>
-      <c r="BQ10" s="34"/>
-      <c r="BR10" s="34"/>
-      <c r="BS10" s="34"/>
-      <c r="BT10" s="35"/>
-      <c r="BU10" s="43"/>
+      <c r="BE10" s="19"/>
+      <c r="BF10" s="20"/>
+      <c r="BG10" s="25"/>
+      <c r="BH10" s="19"/>
+      <c r="BI10" s="19"/>
+      <c r="BJ10" s="19"/>
+      <c r="BK10" s="19"/>
+      <c r="BL10" s="19"/>
+      <c r="BM10" s="19"/>
+      <c r="BN10" s="19"/>
+      <c r="BO10" s="19"/>
+      <c r="BP10" s="19"/>
+      <c r="BQ10" s="19"/>
+      <c r="BR10" s="19"/>
+      <c r="BS10" s="19"/>
+      <c r="BT10" s="20"/>
+      <c r="BU10" s="28"/>
     </row>
     <row r="11" spans="1:73" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="15" t="s">
         <v>27</v>
       </c>
       <c r="B11" t="s">
         <v>28</v>
       </c>
       <c r="C11" s="11"/>
-      <c r="O11" s="34"/>
-      <c r="P11" s="35"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="20"/>
       <c r="Q11" s="11"/>
-      <c r="AQ11" s="34"/>
-      <c r="AR11" s="35"/>
+      <c r="AQ11" s="19"/>
+      <c r="AR11" s="20"/>
       <c r="AS11" s="11"/>
-      <c r="BE11" s="34"/>
-      <c r="BF11" s="35"/>
-      <c r="BG11" s="40"/>
-      <c r="BH11" s="34"/>
-      <c r="BI11" s="34"/>
-      <c r="BJ11" s="34"/>
-      <c r="BK11" s="34"/>
-      <c r="BL11" s="34"/>
-      <c r="BM11" s="34"/>
-      <c r="BN11" s="34"/>
-      <c r="BO11" s="34"/>
-      <c r="BP11" s="34"/>
-      <c r="BQ11" s="34"/>
-      <c r="BR11" s="34"/>
-      <c r="BS11" s="34"/>
-      <c r="BT11" s="35"/>
-      <c r="BU11" s="43"/>
+      <c r="BE11" s="19"/>
+      <c r="BF11" s="20"/>
+      <c r="BG11" s="25"/>
+      <c r="BH11" s="19"/>
+      <c r="BI11" s="19"/>
+      <c r="BJ11" s="19"/>
+      <c r="BK11" s="19"/>
+      <c r="BL11" s="19"/>
+      <c r="BM11" s="19"/>
+      <c r="BN11" s="19"/>
+      <c r="BO11" s="19"/>
+      <c r="BP11" s="19"/>
+      <c r="BQ11" s="19"/>
+      <c r="BR11" s="19"/>
+      <c r="BS11" s="19"/>
+      <c r="BT11" s="20"/>
+      <c r="BU11" s="28"/>
     </row>
     <row r="12" spans="1:73" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="15" t="s">
         <v>29</v>
       </c>
       <c r="B12" t="s">
         <v>28</v>
       </c>
       <c r="C12" s="11"/>
-      <c r="O12" s="34"/>
-      <c r="P12" s="35"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="20"/>
       <c r="Q12" s="11"/>
-      <c r="AQ12" s="34"/>
-      <c r="AR12" s="35"/>
+      <c r="AQ12" s="19"/>
+      <c r="AR12" s="20"/>
       <c r="AS12" s="11"/>
-      <c r="BE12" s="34"/>
-      <c r="BF12" s="35"/>
-      <c r="BG12" s="40"/>
-      <c r="BH12" s="34"/>
-      <c r="BI12" s="34"/>
-      <c r="BJ12" s="34"/>
-      <c r="BK12" s="34"/>
-      <c r="BL12" s="34"/>
-      <c r="BM12" s="34"/>
-      <c r="BN12" s="34"/>
-      <c r="BO12" s="34"/>
-      <c r="BP12" s="34"/>
-      <c r="BQ12" s="34"/>
-      <c r="BR12" s="34"/>
-      <c r="BS12" s="34"/>
-      <c r="BT12" s="35"/>
-      <c r="BU12" s="43"/>
+      <c r="BE12" s="19"/>
+      <c r="BF12" s="20"/>
+      <c r="BG12" s="25"/>
+      <c r="BH12" s="19"/>
+      <c r="BI12" s="19"/>
+      <c r="BJ12" s="19"/>
+      <c r="BK12" s="19"/>
+      <c r="BL12" s="19"/>
+      <c r="BM12" s="19"/>
+      <c r="BN12" s="19"/>
+      <c r="BO12" s="19"/>
+      <c r="BP12" s="19"/>
+      <c r="BQ12" s="19"/>
+      <c r="BR12" s="19"/>
+      <c r="BS12" s="19"/>
+      <c r="BT12" s="20"/>
+      <c r="BU12" s="28"/>
     </row>
     <row r="13" spans="1:73" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="11"/>
-      <c r="O13" s="34"/>
-      <c r="P13" s="35"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="20"/>
       <c r="Q13" s="11"/>
-      <c r="AQ13" s="34"/>
-      <c r="AR13" s="35"/>
+      <c r="AQ13" s="19"/>
+      <c r="AR13" s="20"/>
       <c r="AS13" s="11"/>
-      <c r="BE13" s="34"/>
-      <c r="BF13" s="35"/>
-      <c r="BG13" s="40"/>
-      <c r="BH13" s="34"/>
-      <c r="BI13" s="34"/>
-      <c r="BJ13" s="34"/>
-      <c r="BK13" s="34"/>
-      <c r="BL13" s="34"/>
-      <c r="BM13" s="34"/>
-      <c r="BN13" s="34"/>
-      <c r="BO13" s="34"/>
-      <c r="BP13" s="34"/>
-      <c r="BQ13" s="34"/>
-      <c r="BR13" s="34"/>
-      <c r="BS13" s="34"/>
-      <c r="BT13" s="35"/>
-      <c r="BU13" s="43"/>
+      <c r="BE13" s="19"/>
+      <c r="BF13" s="20"/>
+      <c r="BG13" s="25"/>
+      <c r="BH13" s="19"/>
+      <c r="BI13" s="19"/>
+      <c r="BJ13" s="19"/>
+      <c r="BK13" s="19"/>
+      <c r="BL13" s="19"/>
+      <c r="BM13" s="19"/>
+      <c r="BN13" s="19"/>
+      <c r="BO13" s="19"/>
+      <c r="BP13" s="19"/>
+      <c r="BQ13" s="19"/>
+      <c r="BR13" s="19"/>
+      <c r="BS13" s="19"/>
+      <c r="BT13" s="20"/>
+      <c r="BU13" s="28"/>
     </row>
     <row r="14" spans="1:73" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="11"/>
-      <c r="O14" s="34"/>
-      <c r="P14" s="35"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="20"/>
       <c r="Q14" s="11"/>
-      <c r="AQ14" s="34"/>
-      <c r="AR14" s="35"/>
+      <c r="AQ14" s="19"/>
+      <c r="AR14" s="20"/>
       <c r="AS14" s="11"/>
-      <c r="BE14" s="34"/>
-      <c r="BF14" s="35"/>
-      <c r="BG14" s="40"/>
-      <c r="BH14" s="34"/>
-      <c r="BI14" s="34"/>
-      <c r="BJ14" s="34"/>
-      <c r="BK14" s="34"/>
-      <c r="BL14" s="34"/>
-      <c r="BM14" s="34"/>
-      <c r="BN14" s="34"/>
-      <c r="BO14" s="34"/>
-      <c r="BP14" s="34"/>
-      <c r="BQ14" s="34"/>
-      <c r="BR14" s="34"/>
-      <c r="BS14" s="34"/>
-      <c r="BT14" s="35"/>
-      <c r="BU14" s="43"/>
+      <c r="BE14" s="19"/>
+      <c r="BF14" s="20"/>
+      <c r="BG14" s="25"/>
+      <c r="BH14" s="19"/>
+      <c r="BI14" s="19"/>
+      <c r="BJ14" s="19"/>
+      <c r="BK14" s="19"/>
+      <c r="BL14" s="19"/>
+      <c r="BM14" s="19"/>
+      <c r="BN14" s="19"/>
+      <c r="BO14" s="19"/>
+      <c r="BP14" s="19"/>
+      <c r="BQ14" s="19"/>
+      <c r="BR14" s="19"/>
+      <c r="BS14" s="19"/>
+      <c r="BT14" s="20"/>
+      <c r="BU14" s="28"/>
     </row>
     <row r="15" spans="1:73" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="11"/>
-      <c r="O15" s="34"/>
-      <c r="P15" s="35"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="20"/>
       <c r="Q15" s="11"/>
-      <c r="AQ15" s="34"/>
-      <c r="AR15" s="35"/>
+      <c r="AQ15" s="19"/>
+      <c r="AR15" s="20"/>
       <c r="AS15" s="11"/>
-      <c r="BE15" s="34"/>
-      <c r="BF15" s="35"/>
-      <c r="BG15" s="40"/>
-      <c r="BH15" s="34"/>
-      <c r="BI15" s="34"/>
-      <c r="BJ15" s="34"/>
-      <c r="BK15" s="34"/>
-      <c r="BL15" s="34"/>
-      <c r="BM15" s="34"/>
-      <c r="BN15" s="34"/>
-      <c r="BO15" s="34"/>
-      <c r="BP15" s="34"/>
-      <c r="BQ15" s="34"/>
-      <c r="BR15" s="34"/>
-      <c r="BS15" s="34"/>
-      <c r="BT15" s="35"/>
-      <c r="BU15" s="43"/>
+      <c r="BE15" s="19"/>
+      <c r="BF15" s="20"/>
+      <c r="BG15" s="25"/>
+      <c r="BH15" s="19"/>
+      <c r="BI15" s="19"/>
+      <c r="BJ15" s="19"/>
+      <c r="BK15" s="19"/>
+      <c r="BL15" s="19"/>
+      <c r="BM15" s="19"/>
+      <c r="BN15" s="19"/>
+      <c r="BO15" s="19"/>
+      <c r="BP15" s="19"/>
+      <c r="BQ15" s="19"/>
+      <c r="BR15" s="19"/>
+      <c r="BS15" s="19"/>
+      <c r="BT15" s="20"/>
+      <c r="BU15" s="28"/>
     </row>
     <row r="16" spans="1:73" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="11"/>
-      <c r="O16" s="34"/>
-      <c r="P16" s="35"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="20"/>
       <c r="Q16" s="11"/>
-      <c r="AQ16" s="34"/>
-      <c r="AR16" s="35"/>
+      <c r="AQ16" s="19"/>
+      <c r="AR16" s="20"/>
       <c r="AS16" s="11"/>
-      <c r="BE16" s="34"/>
-      <c r="BF16" s="35"/>
-      <c r="BG16" s="40"/>
-      <c r="BH16" s="34"/>
-      <c r="BI16" s="34"/>
-      <c r="BJ16" s="34"/>
-      <c r="BK16" s="34"/>
-      <c r="BL16" s="34"/>
-      <c r="BM16" s="34"/>
-      <c r="BN16" s="34"/>
-      <c r="BO16" s="34"/>
-      <c r="BP16" s="34"/>
-      <c r="BQ16" s="34"/>
-      <c r="BR16" s="34"/>
-      <c r="BS16" s="34"/>
-      <c r="BT16" s="35"/>
-      <c r="BU16" s="43"/>
+      <c r="BE16" s="19"/>
+      <c r="BF16" s="20"/>
+      <c r="BG16" s="25"/>
+      <c r="BH16" s="19"/>
+      <c r="BI16" s="19"/>
+      <c r="BJ16" s="19"/>
+      <c r="BK16" s="19"/>
+      <c r="BL16" s="19"/>
+      <c r="BM16" s="19"/>
+      <c r="BN16" s="19"/>
+      <c r="BO16" s="19"/>
+      <c r="BP16" s="19"/>
+      <c r="BQ16" s="19"/>
+      <c r="BR16" s="19"/>
+      <c r="BS16" s="19"/>
+      <c r="BT16" s="20"/>
+      <c r="BU16" s="28"/>
     </row>
     <row r="17" spans="3:73" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="11"/>
-      <c r="O17" s="34"/>
-      <c r="P17" s="35"/>
+      <c r="O17" s="19"/>
+      <c r="P17" s="20"/>
       <c r="Q17" s="11"/>
-      <c r="AQ17" s="34"/>
-      <c r="AR17" s="35"/>
+      <c r="AQ17" s="19"/>
+      <c r="AR17" s="20"/>
       <c r="AS17" s="11"/>
-      <c r="BE17" s="34"/>
-      <c r="BF17" s="35"/>
-      <c r="BG17" s="40"/>
-      <c r="BH17" s="34"/>
-      <c r="BI17" s="34"/>
-      <c r="BJ17" s="34"/>
-      <c r="BK17" s="34"/>
-      <c r="BL17" s="34"/>
-      <c r="BM17" s="34"/>
-      <c r="BN17" s="34"/>
-      <c r="BO17" s="34"/>
-      <c r="BP17" s="34"/>
-      <c r="BQ17" s="34"/>
-      <c r="BR17" s="34"/>
-      <c r="BS17" s="34"/>
-      <c r="BT17" s="35"/>
-      <c r="BU17" s="43"/>
+      <c r="BE17" s="19"/>
+      <c r="BF17" s="20"/>
+      <c r="BG17" s="25"/>
+      <c r="BH17" s="19"/>
+      <c r="BI17" s="19"/>
+      <c r="BJ17" s="19"/>
+      <c r="BK17" s="19"/>
+      <c r="BL17" s="19"/>
+      <c r="BM17" s="19"/>
+      <c r="BN17" s="19"/>
+      <c r="BO17" s="19"/>
+      <c r="BP17" s="19"/>
+      <c r="BQ17" s="19"/>
+      <c r="BR17" s="19"/>
+      <c r="BS17" s="19"/>
+      <c r="BT17" s="20"/>
+      <c r="BU17" s="28"/>
     </row>
     <row r="18" spans="3:73" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="11"/>
-      <c r="O18" s="34"/>
-      <c r="P18" s="35"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="20"/>
       <c r="Q18" s="11"/>
-      <c r="AQ18" s="34"/>
-      <c r="AR18" s="35"/>
+      <c r="AQ18" s="19"/>
+      <c r="AR18" s="20"/>
       <c r="AS18" s="11"/>
-      <c r="BE18" s="34"/>
-      <c r="BF18" s="35"/>
-      <c r="BG18" s="40"/>
-      <c r="BH18" s="34"/>
-      <c r="BI18" s="34"/>
-      <c r="BJ18" s="34"/>
-      <c r="BK18" s="34"/>
-      <c r="BL18" s="34"/>
-      <c r="BM18" s="34"/>
-      <c r="BN18" s="34"/>
-      <c r="BO18" s="34"/>
-      <c r="BP18" s="34"/>
-      <c r="BQ18" s="34"/>
-      <c r="BR18" s="34"/>
-      <c r="BS18" s="34"/>
-      <c r="BT18" s="35"/>
-      <c r="BU18" s="43"/>
+      <c r="BE18" s="19"/>
+      <c r="BF18" s="20"/>
+      <c r="BG18" s="25"/>
+      <c r="BH18" s="19"/>
+      <c r="BI18" s="19"/>
+      <c r="BJ18" s="19"/>
+      <c r="BK18" s="19"/>
+      <c r="BL18" s="19"/>
+      <c r="BM18" s="19"/>
+      <c r="BN18" s="19"/>
+      <c r="BO18" s="19"/>
+      <c r="BP18" s="19"/>
+      <c r="BQ18" s="19"/>
+      <c r="BR18" s="19"/>
+      <c r="BS18" s="19"/>
+      <c r="BT18" s="20"/>
+      <c r="BU18" s="28"/>
     </row>
     <row r="19" spans="3:73" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="11"/>
-      <c r="O19" s="34"/>
-      <c r="P19" s="35"/>
+      <c r="O19" s="19"/>
+      <c r="P19" s="20"/>
       <c r="Q19" s="11"/>
-      <c r="AQ19" s="34"/>
-      <c r="AR19" s="35"/>
+      <c r="AQ19" s="19"/>
+      <c r="AR19" s="20"/>
       <c r="AS19" s="11"/>
-      <c r="BE19" s="34"/>
-      <c r="BF19" s="35"/>
-      <c r="BG19" s="40"/>
-      <c r="BH19" s="34"/>
-      <c r="BI19" s="34"/>
-      <c r="BJ19" s="34"/>
-      <c r="BK19" s="34"/>
-      <c r="BL19" s="34"/>
-      <c r="BM19" s="34"/>
-      <c r="BN19" s="34"/>
-      <c r="BO19" s="34"/>
-      <c r="BP19" s="34"/>
-      <c r="BQ19" s="34"/>
-      <c r="BR19" s="34"/>
-      <c r="BS19" s="34"/>
-      <c r="BT19" s="35"/>
-      <c r="BU19" s="43"/>
+      <c r="BE19" s="19"/>
+      <c r="BF19" s="20"/>
+      <c r="BG19" s="25"/>
+      <c r="BH19" s="19"/>
+      <c r="BI19" s="19"/>
+      <c r="BJ19" s="19"/>
+      <c r="BK19" s="19"/>
+      <c r="BL19" s="19"/>
+      <c r="BM19" s="19"/>
+      <c r="BN19" s="19"/>
+      <c r="BO19" s="19"/>
+      <c r="BP19" s="19"/>
+      <c r="BQ19" s="19"/>
+      <c r="BR19" s="19"/>
+      <c r="BS19" s="19"/>
+      <c r="BT19" s="20"/>
+      <c r="BU19" s="28"/>
     </row>
     <row r="20" spans="3:73" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C20" s="12"/>
@@ -1801,8 +1857,8 @@
       <c r="L20" s="13"/>
       <c r="M20" s="13"/>
       <c r="N20" s="13"/>
-      <c r="O20" s="36"/>
-      <c r="P20" s="37"/>
+      <c r="O20" s="21"/>
+      <c r="P20" s="22"/>
       <c r="Q20" s="12"/>
       <c r="R20" s="13"/>
       <c r="S20" s="13"/>
@@ -1829,8 +1885,8 @@
       <c r="AN20" s="13"/>
       <c r="AO20" s="13"/>
       <c r="AP20" s="13"/>
-      <c r="AQ20" s="36"/>
-      <c r="AR20" s="37"/>
+      <c r="AQ20" s="21"/>
+      <c r="AR20" s="22"/>
       <c r="AS20" s="12"/>
       <c r="AT20" s="13"/>
       <c r="AU20" s="13"/>
@@ -1843,31 +1899,26 @@
       <c r="BB20" s="13"/>
       <c r="BC20" s="13"/>
       <c r="BD20" s="13"/>
-      <c r="BE20" s="36"/>
-      <c r="BF20" s="37"/>
-      <c r="BG20" s="41"/>
-      <c r="BH20" s="36"/>
-      <c r="BI20" s="36"/>
-      <c r="BJ20" s="36"/>
-      <c r="BK20" s="36"/>
-      <c r="BL20" s="36"/>
-      <c r="BM20" s="36"/>
-      <c r="BN20" s="36"/>
-      <c r="BO20" s="36"/>
-      <c r="BP20" s="36"/>
-      <c r="BQ20" s="36"/>
-      <c r="BR20" s="36"/>
-      <c r="BS20" s="36"/>
-      <c r="BT20" s="37"/>
-      <c r="BU20" s="44"/>
+      <c r="BE20" s="21"/>
+      <c r="BF20" s="22"/>
+      <c r="BG20" s="26"/>
+      <c r="BH20" s="21"/>
+      <c r="BI20" s="21"/>
+      <c r="BJ20" s="21"/>
+      <c r="BK20" s="21"/>
+      <c r="BL20" s="21"/>
+      <c r="BM20" s="21"/>
+      <c r="BN20" s="21"/>
+      <c r="BO20" s="21"/>
+      <c r="BP20" s="21"/>
+      <c r="BQ20" s="21"/>
+      <c r="BR20" s="21"/>
+      <c r="BS20" s="21"/>
+      <c r="BT20" s="22"/>
+      <c r="BU20" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="O4:P20"/>
-    <mergeCell ref="AQ4:AR20"/>
-    <mergeCell ref="BE4:BF20"/>
-    <mergeCell ref="BG4:BT20"/>
-    <mergeCell ref="BU4:BU20"/>
     <mergeCell ref="BS1:BU1"/>
     <mergeCell ref="C2:P2"/>
     <mergeCell ref="Q2:AD2"/>
@@ -1884,8 +1935,133 @@
     <mergeCell ref="O1:U1"/>
     <mergeCell ref="V1:AB1"/>
     <mergeCell ref="AC1:AI1"/>
+    <mergeCell ref="O4:P20"/>
+    <mergeCell ref="AQ4:AR20"/>
+    <mergeCell ref="BE4:BF20"/>
+    <mergeCell ref="BG4:BT20"/>
+    <mergeCell ref="BU4:BU20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E62F7F27-1A6F-457B-B89F-F142DD0D21DE}">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="141.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="49" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="48" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="48"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="47" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="48"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="47" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="48"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="48"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="48"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="48"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="48"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="48"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="48"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="48"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="48"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="48"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="48"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="48"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="48"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:B16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>